<commit_message>
created array stepdefinition file and log4j file
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/testdata.xlsx
+++ b/src/test/resources/testData/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbehl\eclipse-workspace\com.qa.dsalgo\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8620DE0A-88DC-4174-AA70-D80E09433170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5520126D-6A6C-4170-AB93-79F7D42B0696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{7F2D40C6-60C7-4E4C-9444-6CD5B34C630C}"/>
   </bookViews>
@@ -39,7 +39,7 @@
     <t>username</t>
   </si>
   <si>
-    <t>qatitans19</t>
+    <t>qatitans27</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
created stepdefinition for login and linked list modules
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/testdata.xlsx
+++ b/src/test/resources/testData/testdata.xlsx
@@ -2,18 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbehl\eclipse-workspace\com.qa.dsalgo\src\test\resources\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\madhu\eclipse-workspace\com.qa.dsalgo\Dsalgo-QAtitans\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8620DE0A-88DC-4174-AA70-D80E09433170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6877A774-6A23-445B-852E-11BCAE2868E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{7F2D40C6-60C7-4E4C-9444-6CD5B34C630C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{7F2D40C6-60C7-4E4C-9444-6CD5B34C630C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>1@chicago</t>
   </si>
@@ -40,6 +41,24 @@
   </si>
   <si>
     <t>qatitans19</t>
+  </si>
+  <si>
+    <t>invaliduser1</t>
+  </si>
+  <si>
+    <t>invalidpass</t>
+  </si>
+  <si>
+    <t>invalidpass2</t>
+  </si>
+  <si>
+    <t>invaliduser2</t>
+  </si>
+  <si>
+    <t>isdatavalid</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -440,17 +459,17 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.36328125" customWidth="1"/>
-    <col min="3" max="3" width="14.7265625" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -461,7 +480,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -480,4 +499,62 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C98736-8867-43EA-AAD2-021E9742A3F1}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
created step definiton file for Tree module and updated hooks file
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/testdata.xlsx
+++ b/src/test/resources/testData/testdata.xlsx
@@ -3,16 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{BC551297-8621-441F-A079-EC1C0E139FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbehl\eclipse-workspace\com.qa.dsalgo\src\test\resources\testData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20EA83BC-C52D-4C96-B297-D272FEDAFA14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{7F2D40C6-60C7-4E4C-9444-6CD5B34C630C}"/>
+    <workbookView xWindow="2920" yWindow="2920" windowWidth="14400" windowHeight="8170" xr2:uid="{7F2D40C6-60C7-4E4C-9444-6CD5B34C630C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:U8"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,9 +40,6 @@
     <t>username</t>
   </si>
   <si>
-    <t>qatitans19</t>
-  </si>
-  <si>
     <t>invaliduser1</t>
   </si>
   <si>
@@ -55,6 +56,9 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>qatitans31</t>
   </si>
 </sst>
 </file>
@@ -455,17 +459,17 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="9.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" customWidth="1"/>
+    <col min="3" max="3" width="14.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -476,9 +480,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -501,18 +505,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C98736-8867-43EA-AAD2-021E9742A3F1}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -520,34 +524,34 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>10</v>
+      <c r="C3" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed code for Registration feature
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/testdata.xlsx
+++ b/src/test/resources/testData/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbehl\eclipse-workspace\com.qa.dsalgo\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EBEEC64-0CF7-43E0-8CC5-28D3DCA034C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F36BB186-D089-4D34-9AA1-BD8295C8A568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2920" yWindow="2920" windowWidth="14400" windowHeight="8170" xr2:uid="{7F2D40C6-60C7-4E4C-9444-6CD5B34C630C}"/>
+    <workbookView xWindow="0" yWindow="2640" windowWidth="14400" windowHeight="8170" xr2:uid="{7F2D40C6-60C7-4E4C-9444-6CD5B34C630C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
     <t>N</t>
   </si>
   <si>
-    <t>qatitans37</t>
+    <t>qatitans40</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Fixed Jenkins failures and made changes by Nishi
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/testdata.xlsx
+++ b/src/test/resources/testData/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbehl\eclipse-workspace\com.qa.dsalgo\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F36BB186-D089-4D34-9AA1-BD8295C8A568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879299C6-77A0-4ED3-9EFB-9498C2C23A9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2640" windowWidth="14400" windowHeight="8170" xr2:uid="{7F2D40C6-60C7-4E4C-9444-6CD5B34C630C}"/>
+    <workbookView xWindow="0" yWindow="2640" windowWidth="14400" windowHeight="8170" activeTab="1" xr2:uid="{7F2D40C6-60C7-4E4C-9444-6CD5B34C630C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -459,7 +459,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -505,7 +505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C98736-8867-43EA-AAD2-021E9742A3F1}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Code merged with main.
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/testdata.xlsx
+++ b/src/test/resources/testData/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbehl\eclipse-workspace\com.qa.dsalgo\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20EA83BC-C52D-4C96-B297-D272FEDAFA14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F36BB186-D089-4D34-9AA1-BD8295C8A568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2920" yWindow="2920" windowWidth="14400" windowHeight="8170" xr2:uid="{7F2D40C6-60C7-4E4C-9444-6CD5B34C630C}"/>
+    <workbookView xWindow="0" yWindow="2640" windowWidth="14400" windowHeight="8170" xr2:uid="{7F2D40C6-60C7-4E4C-9444-6CD5B34C630C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
     <t>N</t>
   </si>
   <si>
-    <t>qatitans31</t>
+    <t>qatitans40</t>
   </si>
 </sst>
 </file>
@@ -460,7 +460,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Updated Login, LinkedList, Stack page classes, step definitions, feature files, and test data
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/testdata.xlsx
+++ b/src/test/resources/testData/testdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbehl\eclipse-workspace\com.qa.dsalgo\src\test\resources\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\madhu\eclipse-workspace\com.qa.dsalgo\Dsalgo-QAtitans\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EBEEC64-0CF7-43E0-8CC5-28D3DCA034C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2FCE380-93D5-4AA9-9697-1A3E31B4C113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2920" yWindow="2920" windowWidth="14400" windowHeight="8170" xr2:uid="{7F2D40C6-60C7-4E4C-9444-6CD5B34C630C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7F2D40C6-60C7-4E4C-9444-6CD5B34C630C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>1@chicago</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>qatitans37</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -457,19 +460,21 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96B4B85C-6CFF-44B7-A322-7AEF1732F15F}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D1" sqref="D1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.453125" customWidth="1"/>
-    <col min="3" max="3" width="14.7265625" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -479,8 +484,11 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -489,6 +497,9 @@
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -506,17 +517,17 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -527,7 +538,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -538,7 +549,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -546,7 +557,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Updated files for running reporsts on my local
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/testdata.xlsx
+++ b/src/test/resources/testData/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbehl\eclipse-workspace\com.qa.dsalgo\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879299C6-77A0-4ED3-9EFB-9498C2C23A9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756C0323-B7E3-493F-A49A-6DDB98C9A61E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2640" windowWidth="14400" windowHeight="8170" activeTab="1" xr2:uid="{7F2D40C6-60C7-4E4C-9444-6CD5B34C630C}"/>
+    <workbookView xWindow="0" yWindow="2640" windowWidth="14400" windowHeight="8170" xr2:uid="{7F2D40C6-60C7-4E4C-9444-6CD5B34C630C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
     <t>N</t>
   </si>
   <si>
-    <t>qatitans40</t>
+    <t>qatitans65</t>
   </si>
 </sst>
 </file>
@@ -459,7 +459,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -505,7 +505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1C98736-8867-43EA-AAD2-021E9742A3F1}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Made changes and updated the pom xml
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/testdata.xlsx
+++ b/src/test/resources/testData/testdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbehl\eclipse-workspace\com.qa.dsalgo\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB50218-3946-482D-BA68-EDC04EBDE4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADAAEF99-2FAE-485B-8CA9-804F7ED1ACAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2640" windowWidth="14400" windowHeight="8170" xr2:uid="{7F2D40C6-60C7-4E4C-9444-6CD5B34C630C}"/>
   </bookViews>
@@ -58,10 +58,10 @@
     <t>N</t>
   </si>
   <si>
-    <t>qatitans65</t>
-  </si>
-  <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>qatitans78</t>
   </si>
 </sst>
 </file>
@@ -463,7 +463,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -488,7 +488,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -497,7 +497,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>